<commit_message>
update data in on Aug. 9th, 2020
</commit_message>
<xml_diff>
--- a/data/ershoufang_num_stat.xlsx
+++ b/data/ershoufang_num_stat.xlsx
@@ -388,7 +388,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>11222</v>
+        <v>11395</v>
       </c>
     </row>
     <row r="3">
@@ -401,7 +401,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5946</v>
+        <v>6092</v>
       </c>
     </row>
     <row r="4">
@@ -414,7 +414,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>8895</v>
+        <v>9007</v>
       </c>
     </row>
     <row r="5">
@@ -427,7 +427,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6707</v>
+        <v>6835</v>
       </c>
     </row>
     <row r="6">
@@ -440,7 +440,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5133</v>
+        <v>5243</v>
       </c>
     </row>
     <row r="7">
@@ -453,7 +453,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8283</v>
+        <v>8462</v>
       </c>
     </row>
     <row r="8">
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22417</v>
+        <v>22730</v>
       </c>
     </row>
     <row r="9">
@@ -479,7 +479,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>16561</v>
+        <v>16750</v>
       </c>
     </row>
     <row r="10">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>4974</v>
+        <v>5036</v>
       </c>
     </row>
     <row r="11">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3995</v>
+        <v>3992</v>
       </c>
     </row>
     <row r="12">
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>43</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update app with new data.
</commit_message>
<xml_diff>
--- a/data/ershoufang_num_stat.xlsx
+++ b/data/ershoufang_num_stat.xlsx
@@ -388,7 +388,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>11395</v>
+        <v>11466</v>
       </c>
     </row>
     <row r="3">
@@ -401,7 +401,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>6092</v>
+        <v>6147</v>
       </c>
     </row>
     <row r="4">
@@ -414,7 +414,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9007</v>
+        <v>9155</v>
       </c>
     </row>
     <row r="5">
@@ -427,7 +427,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6835</v>
+        <v>6886</v>
       </c>
     </row>
     <row r="6">
@@ -440,7 +440,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5243</v>
+        <v>5270</v>
       </c>
     </row>
     <row r="7">
@@ -453,7 +453,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8462</v>
+        <v>8567</v>
       </c>
     </row>
     <row r="8">
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22730</v>
+        <v>22879</v>
       </c>
     </row>
     <row r="9">
@@ -479,7 +479,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>16750</v>
+        <v>16927</v>
       </c>
     </row>
     <row r="10">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>5036</v>
+        <v>5087</v>
       </c>
     </row>
     <row r="11">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3992</v>
+        <v>3989</v>
       </c>
     </row>
     <row r="12">
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>